<commit_message>
Four scenarios in the simulation study (pickles with results too large)
</commit_message>
<xml_diff>
--- a/Eichel etal data/elife-52654-fig5-data3.xlsx
+++ b/Eichel etal data/elife-52654-fig5-data3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/Projects/PyCharm/Channel_coexpression/Eichel etal data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/PyCharm/Channel_coexpression/Eichel etal data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF37D57-01A3-3D40-9A3B-05091CF61B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5026F367-9FCF-4443-A884-4019809467C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{CB337B10-F5C1-9742-AD59-80DBAC5DCD01}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{CB337B10-F5C1-9742-AD59-80DBAC5DCD01}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 5d" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
     <t>Ratio</t>
   </si>
   <si>
-    <t>Double coloc nonzero</t>
+    <t>Double coloc removed zeros</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7AF67E-3B6E-E141-AD12-A6D3880B2503}">
   <dimension ref="A3:G269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>